<commit_message>
Misc updates related to Reach Ranking, etc.
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Criteria_Reach_Scoring_Restoration_and_Protection.xlsx
+++ b/Data/Criteria_and_Scoring/Criteria_Reach_Scoring_Restoration_and_Protection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73DBF656-7606-4948-A39A-EB6CB0E5C8C3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E2B37A-F341-43BC-AECE-1DAD5CE35960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1920" yWindow="1452" windowWidth="19992" windowHeight="11508" xr2:uid="{1D4F3EA7-69B3-4B1F-A157-E5A1D08E65AF}"/>
+    <workbookView xWindow="2292" yWindow="1956" windowWidth="19968" windowHeight="10356" xr2:uid="{1D4F3EA7-69B3-4B1F-A157-E5A1D08E65AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79603F0-0E57-4CCE-8F58-4B1744A11D6A}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -613,10 +613,10 @@
         <v>13</v>
       </c>
       <c r="F3">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="G3">
-        <v>70</v>
+        <v>0.8</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -1135,10 +1135,10 @@
         <v>13</v>
       </c>
       <c r="F21">
-        <v>70</v>
+        <v>0.7</v>
       </c>
       <c r="G21">
-        <v>101</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="H21" t="s">
         <v>13</v>

</xml_diff>

<commit_message>
Many edits over the last several months
</commit_message>
<xml_diff>
--- a/Data/Criteria_and_Scoring/Criteria_Reach_Scoring_Restoration_and_Protection.xlsx
+++ b/Data/Criteria_and_Scoring/Criteria_Reach_Scoring_Restoration_and_Protection.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryan\Documents\GitHub\Prioritization_Step2_Data_R_Project\Data\Criteria_and_Scoring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95E2B37A-F341-43BC-AECE-1DAD5CE35960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211E40B6-14E8-499E-BF5F-C143C2ABA5CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2292" yWindow="1956" windowWidth="19968" windowHeight="10356" xr2:uid="{1D4F3EA7-69B3-4B1F-A157-E5A1D08E65AF}"/>
+    <workbookView xWindow="8310" yWindow="-15180" windowWidth="25800" windowHeight="14430" xr2:uid="{1D4F3EA7-69B3-4B1F-A157-E5A1D08E65AF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -129,12 +129,6 @@
     <t>Protection</t>
   </si>
   <si>
-    <t>AU Tier 1 for Protection</t>
-  </si>
-  <si>
-    <t>AU Tier 1 for Restoratoin</t>
-  </si>
-  <si>
     <t>Want high quality for protection</t>
   </si>
   <si>
@@ -160,6 +154,12 @@
   </si>
   <si>
     <t>no adjacent protected area</t>
+  </si>
+  <si>
+    <t>AU Tier 1 or 2 for Protection (put maximum Tier)</t>
+  </si>
+  <si>
+    <t>AU Tier 1 or 2 for Restoration (put maximum Tier)</t>
   </si>
 </sst>
 </file>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F79603F0-0E57-4CCE-8F58-4B1744A11D6A}">
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -581,7 +581,7 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F2" t="s">
         <v>13</v>
@@ -593,7 +593,7 @@
         <v>13</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -622,7 +622,7 @@
         <v>13</v>
       </c>
       <c r="I3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
@@ -680,7 +680,7 @@
         <v>13</v>
       </c>
       <c r="I5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -1103,7 +1103,7 @@
         <v>12</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" t="s">
         <v>13</v>
@@ -1115,7 +1115,7 @@
         <v>13</v>
       </c>
       <c r="I20" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
@@ -1144,7 +1144,7 @@
         <v>13</v>
       </c>
       <c r="I21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -1173,7 +1173,7 @@
         <v>13</v>
       </c>
       <c r="I22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -1231,7 +1231,7 @@
         <v>13</v>
       </c>
       <c r="I24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -1378,7 +1378,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B30" t="s">
         <v>29</v>
@@ -1402,12 +1402,12 @@
         <v>5</v>
       </c>
       <c r="I30" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B31" t="s">
         <v>29</v>
@@ -1431,12 +1431,12 @@
         <v>3</v>
       </c>
       <c r="I31" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
         <v>29</v>
@@ -1460,12 +1460,12 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B33" t="s">
         <v>29</v>
@@ -1477,7 +1477,7 @@
         <v>12</v>
       </c>
       <c r="E33" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F33" t="s">
         <v>13</v>
@@ -1491,7 +1491,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B34" t="s">
         <v>29</v>
@@ -1503,7 +1503,7 @@
         <v>12</v>
       </c>
       <c r="E34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F34" t="s">
         <v>13</v>
@@ -1517,7 +1517,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
@@ -1529,7 +1529,7 @@
         <v>12</v>
       </c>
       <c r="E35" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F35" t="s">
         <v>13</v>

</xml_diff>